<commit_message>
small change to comms doc
</commit_message>
<xml_diff>
--- a/documentation/comms.xlsx
+++ b/documentation/comms.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ebenton\Documents\Genesis\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F64D3F4B-9F44-4F94-B0FD-D103796B3D5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B136AE8-EE34-4330-AAE8-AB42AA64228E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AA77DE67-769D-4241-A446-0A59D555C9A7}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Comms" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -435,7 +435,7 @@
   <dimension ref="B1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
adding fw to the workspace
</commit_message>
<xml_diff>
--- a/documentation/comms.xlsx
+++ b/documentation/comms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ebenton\Documents\Genesis\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BB4785F-57F8-417B-B0DD-4D4DB8E06BD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D60383B1-DD49-45EB-ABC3-ABA2AE3FB75E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AA77DE67-769D-4241-A446-0A59D555C9A7}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="42">
   <si>
     <t>From</t>
   </si>
@@ -120,6 +120,42 @@
   </si>
   <si>
     <t>Some messages above are "tunneled" through the CMS to the TS (Module -&gt; CMS -&gt; Touchscreen). To show this relationship, such messages are in similarly highlighted cells.</t>
+  </si>
+  <si>
+    <t>Operation</t>
+  </si>
+  <si>
+    <t>Let the CMS know the Module's SoC</t>
+  </si>
+  <si>
+    <t>Let the CMS know the Module's temp</t>
+  </si>
+  <si>
+    <t>Let the CMS know the Module's overcharge</t>
+  </si>
+  <si>
+    <t>Let the TS display the Module's SoC</t>
+  </si>
+  <si>
+    <t>Let the TS display the Module's temp</t>
+  </si>
+  <si>
+    <t>Let the TS display the overcharge status</t>
+  </si>
+  <si>
+    <t>Let the TS display the System Status</t>
+  </si>
+  <si>
+    <t>Let the TS display the System Relays Status</t>
+  </si>
+  <si>
+    <t>Let the TS display the Bus Voltage</t>
+  </si>
+  <si>
+    <t>Let the TS display the System's Current</t>
+  </si>
+  <si>
+    <t>Let the TS display the total voltage in the Mods</t>
   </si>
 </sst>
 </file>
@@ -143,7 +179,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -174,28 +210,19 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="12">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -228,17 +255,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -336,55 +352,70 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -702,50 +733,62 @@
   <dimension ref="B1:N15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" style="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="21"/>
-    <col min="5" max="5" width="13.140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="15"/>
+    <col min="5" max="5" width="13.140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="42.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="10" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="F1" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="8"/>
-      <c r="I1" s="9"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
     </row>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="16" t="s">
         <v>16</v>
+      </c>
+      <c r="F2" s="24" t="s">
+        <v>31</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="2" t="s">
@@ -754,19 +797,27 @@
       <c r="I2" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="17" t="s">
         <v>16</v>
+      </c>
+      <c r="F3" s="25" t="s">
+        <v>32</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>19</v>
@@ -777,19 +828,27 @@
       <c r="I3" s="3" t="s">
         <v>20</v>
       </c>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="25" t="s">
+      <c r="E4" s="18" t="s">
         <v>16</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>33</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>27</v>
@@ -800,21 +859,29 @@
       <c r="I4" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="23" t="s">
+      <c r="E5" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="F5" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>23</v>
       </c>
       <c r="H5" s="2" t="s">
@@ -823,152 +890,243 @@
       <c r="I5" s="3" t="s">
         <v>24</v>
       </c>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="20"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="24" t="s">
+      <c r="E6" s="17" t="s">
         <v>14</v>
+      </c>
+      <c r="F6" s="25" t="s">
+        <v>35</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="I6" s="5" t="s">
         <v>26</v>
       </c>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="20"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="25" t="s">
+      <c r="E7" s="18" t="s">
         <v>14</v>
       </c>
+      <c r="F7" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="20"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="23" t="s">
+      <c r="E8" s="16" t="s">
         <v>14</v>
       </c>
+      <c r="F8" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="E9" s="17" t="s">
         <v>14</v>
       </c>
+      <c r="F9" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="20"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="24" t="s">
+      <c r="E10" s="17" t="s">
         <v>14</v>
       </c>
+      <c r="F10" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="20"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="24" t="s">
+      <c r="E11" s="17" t="s">
         <v>14</v>
       </c>
+      <c r="F11" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="20"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="20" t="s">
+      <c r="D12" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E12" s="25" t="s">
+      <c r="E12" s="18" t="s">
         <v>14</v>
       </c>
+      <c r="F12" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="20"/>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="20"/>
+      <c r="M13" s="20"/>
+      <c r="N13" s="20"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
-      <c r="I14" s="27"/>
-      <c r="J14" s="27"/>
-      <c r="K14" s="27"/>
-      <c r="L14" s="27"/>
-      <c r="M14" s="27"/>
-      <c r="N14" s="27"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="31"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="20"/>
+      <c r="N14" s="20"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="26" t="s">
+      <c r="B15" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="26"/>
-      <c r="K15" s="26"/>
-      <c r="L15" s="26"/>
-      <c r="M15" s="26"/>
-      <c r="N15" s="26"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="32"/>
+      <c r="J15" s="32"/>
+      <c r="K15" s="19"/>
+      <c r="L15" s="19"/>
+      <c r="M15" s="19"/>
+      <c r="N15" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B15:N15"/>
-    <mergeCell ref="B14:N14"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="B14:J14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>